<commit_message>
Improve code and data
</commit_message>
<xml_diff>
--- a/regression/data/cubic_reg.xlsx
+++ b/regression/data/cubic_reg.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Chart1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -118,8 +117,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.19526739502003043"/>
-                  <c:y val="-0.64301971122697432"/>
+                  <c:x val="0.19526739502003049"/>
+                  <c:y val="-0.64301971122697454"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -198,40 +197,40 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7410000000000005</c:v>
+                  <c:v>3.7410000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3680000000000012</c:v>
+                  <c:v>4.3680000000000012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8870000000000013</c:v>
+                  <c:v>5.8870000000000013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.304000000000002</c:v>
+                  <c:v>7.304000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.6250000000000018</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.8560000000000008</c:v>
+                  <c:v>7.8560000000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0030000000000001</c:v>
+                  <c:v>8.0030000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0719999999999992</c:v>
+                  <c:v>7.0720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7.069</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.9999999999999991</c:v>
+                  <c:v>5.9999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.8709999999999987</c:v>
+                  <c:v>6.8709999999999987</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6.6879999999999971</c:v>
@@ -243,7 +242,7 @@
                   <c:v>7.1839999999999957</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.8749999999999956</c:v>
+                  <c:v>4.8749999999999956</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>6.5359999999999951</c:v>
@@ -252,29 +251,29 @@
                   <c:v>5.1729999999999947</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.7919999999999936</c:v>
+                  <c:v>5.7919999999999936</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="230426112"/>
-        <c:axId val="230427648"/>
+        <c:axId val="145046144"/>
+        <c:axId val="145252736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="230426112"/>
+        <c:axId val="145046144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230427648"/>
+        <c:crossAx val="145252736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="230427648"/>
+        <c:axId val="145252736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -282,7 +281,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="230426112"/>
+        <c:crossAx val="145046144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -293,31 +292,33 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="265" workbookViewId="0"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668820" cy="6292921"/>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>74887</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>174735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>595149</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>155685</xdr:rowOff>
+    </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -330,7 +331,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:absoluteAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -622,7 +623,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,7 +646,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">(A2-3) * (A2-1) * (A2-5) + 4 + RANDBETWEEN(-1, 1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -655,7 +656,7 @@
       </c>
       <c r="B3" s="3">
         <f t="shared" ref="B3:B20" ca="1" si="0">(A3-3) * (A3-1) * (A3-5) + 4 + RANDBETWEEN(-1, 1)</f>
-        <v>4.7410000000000005</v>
+        <v>3.7410000000000005</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -665,7 +666,7 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3680000000000012</v>
+        <v>4.3680000000000012</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -675,7 +676,7 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8870000000000013</v>
+        <v>5.8870000000000013</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -685,7 +686,7 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.304000000000002</v>
+        <v>7.304000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -705,7 +706,7 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8560000000000008</v>
+        <v>7.8560000000000008</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -715,7 +716,7 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0030000000000001</v>
+        <v>8.0030000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -725,7 +726,7 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0719999999999992</v>
+        <v>7.0720000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -745,7 +746,7 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.9999999999999991</v>
+        <v>5.9999999999999991</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -755,7 +756,7 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8709999999999987</v>
+        <v>6.8709999999999987</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -795,7 +796,7 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8749999999999956</v>
+        <v>4.8749999999999956</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -825,10 +826,11 @@
       </c>
       <c r="B20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7919999999999936</v>
+        <v>5.7919999999999936</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>